<commit_message>
RLB0-master kafka service added in docker-compose.yml
</commit_message>
<xml_diff>
--- a/rlb.xlsx
+++ b/rlb.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="57">
   <si>
     <t>String</t>
   </si>
@@ -121,6 +121,72 @@
   </si>
   <si>
     <t>Arpita</t>
+  </si>
+  <si>
+    <t>createdBy</t>
+  </si>
+  <si>
+    <t>updatedBy</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>Operation</t>
+  </si>
+  <si>
+    <t>Shipment (OC)</t>
+  </si>
+  <si>
+    <t>Core</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>roles</t>
+  </si>
+  <si>
+    <t>List&lt;Role&gt;</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>OrderCreate</t>
+  </si>
+  <si>
+    <t>OrderUpdate</t>
+  </si>
+  <si>
+    <t>OrderCancel</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>DeliveryBoy</t>
+  </si>
+  <si>
+    <t>TeamLead</t>
+  </si>
+  <si>
+    <t>user_role</t>
+  </si>
+  <si>
+    <t>roleId</t>
+  </si>
+  <si>
+    <t>userId</t>
   </si>
 </sst>
 </file>
@@ -136,7 +202,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -146,6 +212,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -203,23 +281,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -234,6 +324,109 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Curved Connector 2"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipV="1">
+          <a:off x="1790700" y="619125"/>
+          <a:ext cx="704850" cy="628650"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 101351"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>38102</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Curved Connector 5"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipV="1">
+          <a:off x="2628902" y="6153150"/>
+          <a:ext cx="990598" cy="257174"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 1923"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -523,214 +716,449 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O13"/>
+  <dimension ref="B1:R39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D1" t="s">
+    <row r="1" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+    </row>
+    <row r="2" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D2" s="3" t="s">
+      <c r="L3" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M3" s="8"/>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="E4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D3" s="4" t="s">
+      <c r="F4" s="11"/>
+      <c r="L4" s="3">
+        <v>1</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="E5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H5" t="s">
         <v>33</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L5" s="3">
+        <v>2</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="6"/>
+      <c r="E6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="13"/>
+      <c r="L6" s="3">
+        <v>3</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="E7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B9" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="11"/>
+      <c r="H9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" s="13"/>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
         <v>34</v>
       </c>
-      <c r="N3" t="s">
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="H17" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" s="11"/>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="H18" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="H19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="H20" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="H22" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="9"/>
-      <c r="D4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="6" t="s">
+    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="H23" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="I23" s="11"/>
+    </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="H24" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="H25" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="8"/>
-      <c r="K4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L4" s="3"/>
-      <c r="N4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="O4" s="3"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="G5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="N5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="O5" s="4" t="s">
+      <c r="I25" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="N6" s="4" t="s">
+    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="H26" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B28" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="9"/>
+      <c r="P28" s="9"/>
+      <c r="Q28" s="9"/>
+      <c r="R28" s="9"/>
+    </row>
+    <row r="30" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B30" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" s="10"/>
+      <c r="E30" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F30" s="10"/>
+      <c r="I30" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="J30" s="10"/>
+    </row>
+    <row r="31" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B31" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B32" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F34" s="10"/>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E35" s="3">
         <v>1</v>
       </c>
-      <c r="O6" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="D7" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="N7" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="O7" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="4" t="s">
+      <c r="F35" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E36" s="3">
         <v>2</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="8"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E9" s="4" t="s">
+      <c r="F36" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E37" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>12</v>
-      </c>
+      <c r="F37" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E38" s="3">
+        <v>4</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="K4:L4"/>
+  <mergeCells count="13">
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="B1:R1"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="B28:R28"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="I30:J30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>